<commit_message>
Updated real scores with excel changes
</commit_message>
<xml_diff>
--- a/Wednesday Night Sidepots - MASTER COPY DO NOT EDIT.xlsx
+++ b/Wednesday Night Sidepots - MASTER COPY DO NOT EDIT.xlsx
@@ -9126,17 +9126,17 @@
     <row r="2">
       <c r="A2" s="66" t="inlineStr">
         <is>
-          <t>ALYSSA MILLS</t>
+          <t>ALLEN P. SUMNER</t>
         </is>
       </c>
       <c r="B2" s="66" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>bk201</t>
         </is>
       </c>
       <c r="C2" s="66" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F2" s="257" t="inlineStr">
@@ -9151,17 +9151,17 @@
     <row r="3" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="66" t="inlineStr">
         <is>
-          <t>ANDY COX</t>
+          <t>ANDREW BENTLEY</t>
         </is>
       </c>
       <c r="B3" s="66" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>bk194</t>
         </is>
       </c>
       <c r="C3" s="66" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>32</t>
         </is>
       </c>
       <c r="F3" s="239" t="n"/>
@@ -9170,12 +9170,12 @@
     <row r="4" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="66" t="inlineStr">
         <is>
-          <t>ANTHONY BILLIPS</t>
+          <t>ANTHONY D. BILLIPS</t>
         </is>
       </c>
       <c r="B4" s="66" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>bk202</t>
         </is>
       </c>
       <c r="C4" s="66" t="inlineStr">
@@ -9195,255 +9195,255 @@
     <row r="5">
       <c r="A5" s="66" t="inlineStr">
         <is>
-          <t>ANTHONY WALKER</t>
+          <t>ANTHONY WHITE</t>
         </is>
       </c>
       <c r="B5" s="66" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>bk204</t>
         </is>
       </c>
       <c r="C5" s="66" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="66" t="inlineStr">
         <is>
-          <t>BEN HALL</t>
+          <t>ARTHUR LUCIA</t>
         </is>
       </c>
       <c r="B6" s="66" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>bk181</t>
         </is>
       </c>
       <c r="C6" s="66" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>44</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="66" t="inlineStr">
         <is>
-          <t>BOB BENTLEY</t>
+          <t>AUSTIN TAYLOR</t>
         </is>
       </c>
       <c r="B7" s="66" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>108</t>
         </is>
       </c>
       <c r="C7" s="66" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>109</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="66" t="inlineStr">
         <is>
-          <t>BRAD PHILLIPS</t>
+          <t>BRANDON BOOTH</t>
         </is>
       </c>
       <c r="B8" s="66" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>bk195</t>
         </is>
       </c>
       <c r="C8" s="66" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>31</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="66" t="inlineStr">
         <is>
-          <t>BRANDON BOOTH</t>
+          <t>BRIAN COLEMAN</t>
         </is>
       </c>
       <c r="B9" s="66" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>200</t>
         </is>
       </c>
       <c r="C9" s="66" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>27</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="66" t="inlineStr">
         <is>
-          <t>BRIAN DERKAY</t>
+          <t>BRIAN GRIFFIN</t>
         </is>
       </c>
       <c r="B10" s="66" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>bk188</t>
         </is>
       </c>
       <c r="C10" s="66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>37</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="66" t="inlineStr">
         <is>
-          <t>BRITTNEY STIKE</t>
+          <t>BRIAN K. DICKERSON</t>
         </is>
       </c>
       <c r="B11" s="66" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>bk160</t>
         </is>
       </c>
       <c r="C11" s="66" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>63</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="66" t="inlineStr">
         <is>
-          <t>CAYLA HICKS</t>
+          <t>BUCK WADE</t>
         </is>
       </c>
       <c r="B12" s="66" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>bk157</t>
         </is>
       </c>
       <c r="C12" s="66" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>65</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="66" t="inlineStr">
         <is>
-          <t>COREY WEBB</t>
+          <t>CHARLES E. COLLINS JR.</t>
         </is>
       </c>
       <c r="B13" s="66" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>bk216</t>
         </is>
       </c>
       <c r="C13" s="66" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="66" t="inlineStr">
         <is>
-          <t>CRISSY DERKAY</t>
+          <t>CHRIS SYMANOSKIE</t>
         </is>
       </c>
       <c r="B14" s="66" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>bk157</t>
         </is>
       </c>
       <c r="C14" s="66" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="66" t="inlineStr">
         <is>
-          <t>DANIEL ALDRIDGE</t>
+          <t>CHRISTOPHER C. EASTRIDGE</t>
         </is>
       </c>
       <c r="B15" s="66" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>bk218</t>
         </is>
       </c>
       <c r="C15" s="66" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="66" t="inlineStr">
         <is>
-          <t>DANIELLE PERDUE</t>
+          <t>DAN BIERTZER</t>
         </is>
       </c>
       <c r="B16" s="66" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C16" s="66" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>71</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="66" t="inlineStr">
         <is>
-          <t>DANNY PERDUE</t>
+          <t>DANNY R. LEE</t>
         </is>
       </c>
       <c r="B17" s="66" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>bk183</t>
         </is>
       </c>
       <c r="C17" s="66" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>42</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="66" t="inlineStr">
         <is>
-          <t>DAVID L. EDWARDS</t>
+          <t>DAVID A. WADE</t>
         </is>
       </c>
       <c r="B18" s="66" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>bk201</t>
         </is>
       </c>
       <c r="C18" s="66" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>26</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="66" t="inlineStr">
         <is>
-          <t>DAVID WADE</t>
+          <t>DAVID J. HOWELL</t>
         </is>
       </c>
       <c r="B19" s="66" t="inlineStr">
         <is>
-          <t>bk190</t>
+          <t>bk201</t>
         </is>
       </c>
       <c r="C19" s="66" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D19" s="72" t="n"/>
@@ -9451,697 +9451,697 @@
     <row r="20">
       <c r="A20" s="101" t="inlineStr">
         <is>
-          <t>DENNIS JACQUINTA</t>
+          <t>DYLAN LINKOUS</t>
         </is>
       </c>
       <c r="B20" s="101" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>bk209</t>
         </is>
       </c>
       <c r="C20" s="101" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="101" t="inlineStr">
         <is>
-          <t>DEVIN DURHAM</t>
+          <t>EDWIN G. STIKE</t>
         </is>
       </c>
       <c r="B21" s="101" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>bk184</t>
         </is>
       </c>
       <c r="C21" s="101" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>41</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="101" t="inlineStr">
         <is>
-          <t>DONALD ECKLES</t>
+          <t>GARRY W. MARION</t>
         </is>
       </c>
       <c r="B22" s="101" t="inlineStr">
         <is>
-          <t>242</t>
+          <t>bk208</t>
         </is>
       </c>
       <c r="C22" s="101" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>19</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="101" t="inlineStr">
         <is>
-          <t>DONALD GAMBLIN</t>
+          <t>GLEN LINKOUS</t>
         </is>
       </c>
       <c r="B23" s="101" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>bk191</t>
         </is>
       </c>
       <c r="C23" s="101" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>35</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="101" t="inlineStr">
         <is>
-          <t>EDDIE STIKE</t>
+          <t>JACOB RATCLIFF</t>
         </is>
       </c>
       <c r="B24" s="101" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>bk204</t>
         </is>
       </c>
       <c r="C24" s="101" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>23</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="101" t="inlineStr">
         <is>
-          <t>ERNEST STUBBS</t>
+          <t>JAMES E. RAINEY</t>
         </is>
       </c>
       <c r="B25" s="101" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>bk214</t>
         </is>
       </c>
       <c r="C25" s="101" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>14</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="101" t="inlineStr">
         <is>
-          <t>GARY ROSS</t>
+          <t>JAMES E. SMITH JR.</t>
         </is>
       </c>
       <c r="B26" s="101" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>bk186</t>
         </is>
       </c>
       <c r="C26" s="101" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>39</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="101" t="inlineStr">
         <is>
-          <t>GLENN LINKOUS</t>
+          <t>JEFF STCLAIR</t>
         </is>
       </c>
       <c r="B27" s="101" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>bk191</t>
         </is>
       </c>
       <c r="C27" s="101" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>35</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="101" t="inlineStr">
         <is>
-          <t>HAROLD PHILLIPS</t>
+          <t>JOHN HUNT JR</t>
         </is>
       </c>
       <c r="B28" s="101" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>bk198</t>
         </is>
       </c>
       <c r="C28" s="101" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>28</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="101" t="inlineStr">
         <is>
-          <t>HEATH KELLY</t>
+          <t>JOHNNY W. DICKERSON JR.</t>
         </is>
       </c>
       <c r="B29" s="101" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>bk211</t>
         </is>
       </c>
       <c r="C29" s="101" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="101" t="inlineStr">
         <is>
-          <t>HUNTER WILEY</t>
+          <t>Jamie McGlothlin</t>
         </is>
       </c>
       <c r="B30" s="101" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>188</t>
         </is>
       </c>
       <c r="C30" s="101" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>37</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="101" t="inlineStr">
         <is>
-          <t>JACOB RATCLIFF</t>
+          <t>KRIS RAMEY</t>
         </is>
       </c>
       <c r="B31" s="101" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>bk186</t>
         </is>
       </c>
       <c r="C31" s="101" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>39</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="101" t="inlineStr">
         <is>
-          <t>JARED MEEK</t>
+          <t>LARRY DOSS</t>
         </is>
       </c>
       <c r="B32" s="101" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>bk192</t>
         </is>
       </c>
       <c r="C32" s="101" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>34</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="101" t="inlineStr">
         <is>
-          <t>JEREMY HODGE</t>
+          <t>LARRY E. THOMAS</t>
         </is>
       </c>
       <c r="B33" s="101" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>bk213</t>
         </is>
       </c>
       <c r="C33" s="101" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>15</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="101" t="inlineStr">
         <is>
-          <t>JOHN JARRELS</t>
+          <t>LEE MARSHALL</t>
         </is>
       </c>
       <c r="B34" s="101" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>bk164</t>
         </is>
       </c>
       <c r="C34" s="101" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>59</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="101" t="inlineStr">
         <is>
-          <t>JOHN PERFATER (RIGHT)</t>
+          <t>LUKE LISKA</t>
         </is>
       </c>
       <c r="B35" s="101" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>bk194</t>
         </is>
       </c>
       <c r="C35" s="101" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>32</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="101" t="inlineStr">
         <is>
-          <t>JORDAN LINKOUS</t>
+          <t>MARK D. McGHEE</t>
         </is>
       </c>
       <c r="B36" s="101" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>bk209</t>
         </is>
       </c>
       <c r="C36" s="101" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="101" t="inlineStr">
         <is>
-          <t>JOSH ALBERT</t>
+          <t>MARK UNDERWOOD</t>
         </is>
       </c>
       <c r="B37" s="101" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>bk205</t>
         </is>
       </c>
       <c r="C37" s="101" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>22</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="101" t="inlineStr">
         <is>
-          <t>JOSH ALLEN</t>
+          <t>MASON D. LEE</t>
         </is>
       </c>
       <c r="B38" s="101" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>bk211</t>
         </is>
       </c>
       <c r="C38" s="101" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="101" t="inlineStr">
         <is>
-          <t>JUSTIN MATHEWS</t>
+          <t>MICHAEL D. PHILLIPS</t>
         </is>
       </c>
       <c r="B39" s="101" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>bk185</t>
         </is>
       </c>
       <c r="C39" s="101" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="101" t="inlineStr">
         <is>
-          <t>KARLA P. GRAGG</t>
+          <t>MICHAEL S. ANDERS</t>
         </is>
       </c>
       <c r="B40" s="101" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>bk218</t>
         </is>
       </c>
       <c r="C40" s="101" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="101" t="inlineStr">
         <is>
-          <t>KERRY E. HAMBLIN</t>
+          <t>MOHAMMED ISSA</t>
         </is>
       </c>
       <c r="B41" s="101" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>bk186</t>
         </is>
       </c>
       <c r="C41" s="101" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>39</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="101" t="inlineStr">
         <is>
-          <t>KEVIN DOTSON</t>
+          <t>NAT KESLING</t>
         </is>
       </c>
       <c r="B42" s="101" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>bk224</t>
         </is>
       </c>
       <c r="C42" s="101" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="101" t="inlineStr">
         <is>
-          <t>KIM BOOTH</t>
+          <t>NICHOLAS NEEL</t>
         </is>
       </c>
       <c r="B43" s="101" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>bk196</t>
         </is>
       </c>
       <c r="C43" s="101" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>30</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="101" t="inlineStr">
         <is>
-          <t>KIM HODGE</t>
+          <t>PETE WEBSTER</t>
         </is>
       </c>
       <c r="B44" s="101" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>bk206</t>
         </is>
       </c>
       <c r="C44" s="101" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>21</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="101" t="inlineStr">
         <is>
-          <t>LANDON LAWSON</t>
+          <t>RICHARD BLEVINS</t>
         </is>
       </c>
       <c r="B45" s="101" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>bk182</t>
         </is>
       </c>
       <c r="C45" s="101" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>43</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="101" t="inlineStr">
         <is>
-          <t>LANE ROBERSON</t>
+          <t>ROB HOWELL</t>
         </is>
       </c>
       <c r="B46" s="101" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>bk224</t>
         </is>
       </c>
       <c r="C46" s="101" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="101" t="inlineStr">
         <is>
-          <t>LANNY BELCHER</t>
+          <t>ROLAND S. WRIGHT JR.</t>
         </is>
       </c>
       <c r="B47" s="101" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>bk204</t>
         </is>
       </c>
       <c r="C47" s="101" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>23</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="101" t="inlineStr">
         <is>
-          <t>LARRY RICHARDSON</t>
+          <t>RONNIE E. DUNCAN</t>
         </is>
       </c>
       <c r="B48" s="101" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>bk184</t>
         </is>
       </c>
       <c r="C48" s="101" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>41</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="101" t="inlineStr">
         <is>
-          <t>LEVONNE WALLACE</t>
+          <t>Richard Fairley</t>
         </is>
       </c>
       <c r="B49" s="101" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>bk224</t>
         </is>
       </c>
       <c r="C49" s="101" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="101" t="inlineStr">
         <is>
-          <t>LINDA RAMSEY</t>
+          <t>Ronnie Horton</t>
         </is>
       </c>
       <c r="B50" s="101" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>208</t>
         </is>
       </c>
       <c r="C50" s="101" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>19</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="101" t="inlineStr">
         <is>
-          <t>LUKAS MCGUIRE</t>
+          <t>SCOTT J. BRADLEY</t>
         </is>
       </c>
       <c r="B51" s="101" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>bk205</t>
         </is>
       </c>
       <c r="C51" s="101" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>22</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="101" t="inlineStr">
         <is>
-          <t>MARCIA L. MEADOWS</t>
+          <t>STEWART L. BROWN</t>
         </is>
       </c>
       <c r="B52" s="101" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>bk211</t>
         </is>
       </c>
       <c r="C52" s="101" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="101" t="inlineStr">
         <is>
-          <t>MARIE TEANY</t>
+          <t>Steve Hollandsworth</t>
         </is>
       </c>
       <c r="B53" s="101" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>bk224</t>
         </is>
       </c>
       <c r="C53" s="101" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="101" t="inlineStr">
         <is>
-          <t>MARK C. FLYNN</t>
+          <t>TERRY W. STIKE</t>
         </is>
       </c>
       <c r="B54" s="101" t="inlineStr">
         <is>
-          <t>161</t>
+          <t>bk205</t>
         </is>
       </c>
       <c r="C54" s="101" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>22</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MARK D. McGHEE</t>
+          <t>TODD JONES</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>bk215</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MARK DIXON</t>
+          <t>TRAVIS W. FOUTZ</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>bk207</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>20</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MARK UNDERWOOD</t>
+          <t>TROY W. HURST</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>bk197</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>29</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MATT MCCOY</t>
+          <t>TYLER GRAHAM</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>bk214</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>14</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MICHAEL D. PHILLIPS</t>
+          <t>TYLER MORGAN</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>bk204</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>23</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MICHAEL NEEL</t>
+          <t>WILLIAM L. DONATHAN</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>bk202</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>25</t>
         </is>
       </c>
     </row>

</xml_diff>